<commit_message>
Manier van kolommen lezen van MaccsBox aangepast.
</commit_message>
<xml_diff>
--- a/backend/uploads/percentages.xlsx
+++ b/backend/uploads/percentages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Administratie\2025\Twinfield converter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8530AF39-8A2A-4C42-9615-FDAF47C6B51B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF2B9278-1F78-4DF6-92DC-60CDF0206099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{42E38834-07A5-459D-840C-2DAC20EFC7F2}"/>
   </bookViews>
@@ -2111,14 +2111,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D805CB4-CBC4-44F3-92E5-453EA76FB6BE}">
   <dimension ref="A1:H2516"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2454" workbookViewId="0">
-      <selection activeCell="H2490" sqref="H2490"/>
+    <sheetView tabSelected="1" topLeftCell="A2394" workbookViewId="0">
+      <selection activeCell="C2512" sqref="C2512"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.42578125" style="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="52.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" style="1" customWidth="1"/>
     <col min="4" max="16384" width="16.28515625" style="1"/>
   </cols>

</xml_diff>